<commit_message>
Add RAW and Z similarity outputs with null distributions and heatmaps
Includes cortex/subcortex RAW metrics, permutation nulls, updated z-scores,
and significance-masked heatmaps for adults and adolescents.
</commit_message>
<xml_diff>
--- a/data/raw/PSY_age_of_onset.xlsx
+++ b/data/raw/PSY_age_of_onset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\Git_META\META\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE17DBAA-DBFF-4401-A51F-FDFC8FCD1CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9CA933-F257-4A0C-8B72-1A6DF8B77227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="1905" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -60,10 +60,10 @@
     <t>CHR</t>
   </si>
   <si>
-    <t>Schizotypic</t>
-  </si>
-  <si>
     <t>PTSD</t>
+  </si>
+  <si>
+    <t>Schizotypy</t>
   </si>
 </sst>
 </file>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>20</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>15.5</v>

</xml_diff>